<commit_message>
docs(project_design): update project design
</commit_message>
<xml_diff>
--- a/project_design/project_design.xlsx
+++ b/project_design/project_design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Develop\my-study-note\project_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F4AA74-6BCC-4329-8EA5-F8E1D04D8BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A522BA-41F8-4E23-BBBE-A43208B97A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{C60A6398-7BE2-4883-A906-74D347AFAF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="282">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -395,15 +395,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Bank/name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fetchBanks
-createSeller()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>콘텐츠 이용약관</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -500,10 +491,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Product/name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Product/detail</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -667,14 +654,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상세정보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상세정보 내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>텍스트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -683,10 +662,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Product/details</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>자료후기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -723,10 +698,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Review/details</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Product/reviewId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -751,10 +722,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Inquiry/details</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Inquiry/answer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -779,10 +746,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>모모노트(판매자 이름)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>판매자 스토어</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -847,23 +810,251 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>제목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담은날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.10.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체크박스(개별상품)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cart/createdAt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>총 자료 금액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>규정 동의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>본인은 저작물을 등록~~(약관)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>체크박스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>동의하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서약서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저작권 규정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일선택(버튼)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1학년 1학기 국어 필기.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최대 용량 100MB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록 가능한 파일 형식: pdf, hwp, …</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>제목</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>담은날짜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024.10.03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>금액</t>
+    <t>자료의 내용을 대표할 수 있도록 구체적..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제목 입력창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 카테고리 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학년 카테고리 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 카테고리 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>텍스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입력창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매가격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매가격 입력창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저작시기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연도 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태그</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태그 입력창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태그 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 태그</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세정보 입력(선택)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소개글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자료에 대한 소개글을 입력해주세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소개글 입력창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구성단계별 목차를 입력해주세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목차 입력창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>임시저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택 자료 구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fetchProducts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fetchProduct(productId)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createSeller(정산자유형, 계약자명, 정산자명, 주민번호, 은행, 계좌번호)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>텍스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1(페이지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -871,56 +1062,96 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>체크박스(개별상품)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cart/name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cart/price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cart/createdAt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>총 자료 금액</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20,000원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>선택 자료 결제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 등록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>카테고리 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>과목 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>학년 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상세 내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1(페이지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product/title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1학년</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2004년</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8월</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태그 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1단원. … 2단원. …</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목차 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다윈노트(판매자 이름)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1단원. … 2단원. …</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product/contents</t>
+  </si>
+  <si>
+    <t>fetchCategorySelect
+createProduct(fileLink?, title, categoryId?, price, 저작시기, tagId, detail, contents)
+createCategory(all, grage, subjects)
+createTag(tags[])</t>
+  </si>
+  <si>
+    <t>Product/detail</t>
+  </si>
+  <si>
+    <t>Review/detail</t>
+  </si>
+  <si>
+    <t>Inquiry/detail</t>
+  </si>
+  <si>
+    <t>fetchCategorySelect
+createProduct(fileLink?, title, categoryId?, price, 저작시기, tagId, detail, 목차)
+createCategory(all, grage, subjects)
+createTag(tags[])</t>
   </si>
 </sst>
 </file>
@@ -1313,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430947C9-B8B0-4DE3-877D-B69BC3F0167A}">
-  <dimension ref="B2:G195"/>
+  <dimension ref="B2:G335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="C168" sqref="C168"/>
+    <sheetView tabSelected="1" topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2086,10 +2317,10 @@
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>73</v>
@@ -2101,13 +2332,13 @@
         <v>69</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" s="3"/>
       <c r="C56" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>69</v>
@@ -2116,14 +2347,14 @@
         <v>91</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G56" s="5"/>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" s="3"/>
       <c r="C57" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>73</v>
@@ -2139,10 +2370,10 @@
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" s="3"/>
       <c r="C58" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>69</v>
@@ -2155,7 +2386,7 @@
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" s="3"/>
       <c r="C59" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>73</v>
@@ -2171,7 +2402,7 @@
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60" s="3"/>
       <c r="C60" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>73</v>
@@ -2187,7 +2418,7 @@
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" s="3"/>
       <c r="C61" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>78</v>
@@ -2203,7 +2434,7 @@
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" s="3"/>
       <c r="C62" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>78</v>
@@ -2219,7 +2450,7 @@
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" s="3"/>
       <c r="C63" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>73</v>
@@ -2228,14 +2459,14 @@
         <v>91</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G63" s="5"/>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64" s="3"/>
       <c r="C64" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>73</v>
@@ -2251,7 +2482,7 @@
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" s="3"/>
       <c r="C65" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>78</v>
@@ -2267,7 +2498,7 @@
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" s="3"/>
       <c r="C66" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>78</v>
@@ -2283,7 +2514,7 @@
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" s="3"/>
       <c r="C67" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>73</v>
@@ -2292,14 +2523,14 @@
         <v>91</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G67" s="5"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" s="3"/>
       <c r="C68" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>90</v>
@@ -2314,7 +2545,7 @@
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>72</v>
@@ -2329,7 +2560,7 @@
         <v>69</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>93</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
@@ -2468,6 +2699,9 @@
       <c r="D79" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E79" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="G79" s="3"/>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.3">
@@ -2495,10 +2729,10 @@
         <v>89</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>91</v>
+        <v>9</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="G81" s="3"/>
     </row>
@@ -2552,7 +2786,7 @@
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
-        <v>110</v>
+        <v>204</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>63</v>
@@ -2566,7 +2800,9 @@
       <c r="F86" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G86" s="3"/>
+      <c r="G86" s="4" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B87" s="3"/>
@@ -2619,10 +2855,10 @@
     <row r="90" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B90" s="3"/>
       <c r="C90" s="1" t="s">
-        <v>56</v>
+        <v>204</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>20</v>
+        <v>223</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>9</v>
@@ -2635,10 +2871,10 @@
     <row r="91" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B91" s="3"/>
       <c r="C91" s="1" t="s">
-        <v>58</v>
+        <v>205</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>20</v>
+        <v>223</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>9</v>
@@ -2651,26 +2887,20 @@
     <row r="92" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B92" s="3"/>
       <c r="C92" s="1" t="s">
-        <v>57</v>
+        <v>206</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>9</v>
+        <v>223</v>
       </c>
       <c r="G92" s="3"/>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B93" s="3"/>
       <c r="C93" s="1" t="s">
-        <v>59</v>
+        <v>207</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>20</v>
+        <v>207</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>9</v>
@@ -2683,10 +2913,10 @@
     <row r="94" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B94" s="3"/>
       <c r="C94" s="1" t="s">
-        <v>60</v>
+        <v>208</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>20</v>
+        <v>223</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>9</v>
@@ -2699,10 +2929,10 @@
     <row r="95" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B95" s="3"/>
       <c r="C95" s="1" t="s">
-        <v>61</v>
+        <v>209</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>20</v>
+        <v>224</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>9</v>
@@ -2715,10 +2945,10 @@
     <row r="96" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B96" s="3"/>
       <c r="C96" s="1" t="s">
-        <v>111</v>
+        <v>210</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>20</v>
+        <v>224</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>9</v>
@@ -2731,204 +2961,218 @@
     <row r="97" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B97" s="3"/>
       <c r="C97" s="1" t="s">
-        <v>112</v>
+        <v>211</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="G97" s="3"/>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B98" s="3"/>
       <c r="C98" s="1" t="s">
-        <v>142</v>
+        <v>212</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>115</v>
+        <v>224</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="G98" s="3"/>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B99" s="3"/>
       <c r="C99" s="1" t="s">
-        <v>132</v>
+        <v>213</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="G99" s="3"/>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B100" s="3"/>
       <c r="C100" s="1" t="s">
-        <v>134</v>
+        <v>214</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="G100" s="3"/>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B101" s="3"/>
       <c r="C101" s="1" t="s">
-        <v>131</v>
+        <v>215</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>125</v>
+        <v>9</v>
       </c>
       <c r="G101" s="3"/>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B102" s="3"/>
       <c r="C102" s="1" t="s">
-        <v>133</v>
+        <v>216</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="G102" s="3"/>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B103" s="3"/>
       <c r="C103" s="1" t="s">
-        <v>135</v>
+        <v>217</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="G103" s="3"/>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B104" s="3"/>
       <c r="C104" s="1" t="s">
-        <v>137</v>
+        <v>218</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>20</v>
+        <v>225</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>163</v>
+        <v>9</v>
       </c>
       <c r="G104" s="3"/>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B105" s="3"/>
       <c r="C105" s="1" t="s">
-        <v>136</v>
+        <v>219</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>122</v>
+        <v>9</v>
       </c>
       <c r="G105" s="3"/>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B106" s="3"/>
       <c r="C106" s="1" t="s">
-        <v>138</v>
+        <v>220</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>20</v>
+        <v>226</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>116</v>
+        <v>247</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>124</v>
+        <v>247</v>
       </c>
       <c r="G106" s="3"/>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B107" s="3"/>
       <c r="C107" s="1" t="s">
-        <v>139</v>
+        <v>221</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>140</v>
+        <v>226</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>114</v>
+        <v>247</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>114</v>
+        <v>247</v>
       </c>
       <c r="G107" s="3"/>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B108" s="3"/>
       <c r="C108" s="1" t="s">
-        <v>141</v>
+        <v>222</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>20</v>
+        <v>226</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>116</v>
+        <v>247</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>123</v>
+        <v>247</v>
       </c>
       <c r="G108" s="3"/>
     </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B109" s="3"/>
+      <c r="C109" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G109" s="3"/>
+    </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B110" s="3" t="s">
-        <v>126</v>
-      </c>
+      <c r="B110" s="3"/>
       <c r="C110" s="1" t="s">
-        <v>63</v>
+        <v>228</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>9</v>
@@ -2941,7 +3185,7 @@
     <row r="111" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B111" s="3"/>
       <c r="C111" s="1" t="s">
-        <v>54</v>
+        <v>229</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>20</v>
@@ -2957,10 +3201,10 @@
     <row r="112" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B112" s="3"/>
       <c r="C112" s="1" t="s">
-        <v>52</v>
+        <v>230</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>20</v>
+        <v>226</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>9</v>
@@ -2973,10 +3217,10 @@
     <row r="113" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B113" s="3"/>
       <c r="C113" s="1" t="s">
-        <v>53</v>
+        <v>231</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>20</v>
+        <v>226</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>9</v>
@@ -2989,984 +3233,2583 @@
     <row r="114" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B114" s="3"/>
       <c r="C114" s="1" t="s">
-        <v>127</v>
+        <v>232</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="G114" s="3"/>
     </row>
     <row r="115" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B115" s="3"/>
       <c r="C115" s="1" t="s">
-        <v>128</v>
+        <v>233</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>20</v>
+        <v>225</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>147</v>
+        <v>9</v>
       </c>
       <c r="G115" s="3"/>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B116" s="3"/>
       <c r="C116" s="1" t="s">
-        <v>129</v>
+        <v>234</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>20</v>
+        <v>224</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>147</v>
+        <v>9</v>
       </c>
       <c r="G116" s="3"/>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B117" s="3"/>
       <c r="C117" s="1" t="s">
-        <v>130</v>
+        <v>235</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>147</v>
+        <v>9</v>
       </c>
       <c r="G117" s="3"/>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B118" s="3"/>
       <c r="C118" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="G118" s="3"/>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B119" s="3"/>
       <c r="C119" s="1" t="s">
-        <v>144</v>
+        <v>236</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>20</v>
+        <v>223</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>146</v>
+        <v>9</v>
       </c>
       <c r="G119" s="3"/>
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B120" s="3"/>
       <c r="C120" s="1" t="s">
-        <v>145</v>
+        <v>237</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>20</v>
+        <v>223</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="G120" s="3"/>
     </row>
     <row r="121" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B121" s="3"/>
       <c r="C121" s="1" t="s">
-        <v>149</v>
+        <v>238</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>163</v>
+        <v>9</v>
       </c>
       <c r="G121" s="3"/>
     </row>
     <row r="122" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B122" s="3"/>
       <c r="C122" s="1" t="s">
-        <v>150</v>
+        <v>239</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>20</v>
+        <v>225</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="G122" s="3"/>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B123" s="3"/>
       <c r="C123" s="1" t="s">
-        <v>151</v>
+        <v>240</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>122</v>
+        <v>9</v>
       </c>
       <c r="G123" s="3"/>
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B124" s="3"/>
       <c r="C124" s="1" t="s">
-        <v>153</v>
+        <v>241</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>154</v>
+        <v>223</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="G124" s="3"/>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B125" s="3"/>
       <c r="C125" s="1" t="s">
-        <v>155</v>
+        <v>242</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>154</v>
+        <v>225</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="G125" s="3"/>
     </row>
     <row r="126" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B126" s="3"/>
       <c r="C126" s="1" t="s">
-        <v>159</v>
+        <v>245</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>157</v>
+        <v>224</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>158</v>
+        <v>9</v>
       </c>
       <c r="G126" s="3"/>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B127" s="3"/>
       <c r="C127" s="1" t="s">
-        <v>160</v>
+        <v>243</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>154</v>
+        <v>224</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="G127" s="3"/>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B128" s="3"/>
       <c r="C128" s="1" t="s">
-        <v>161</v>
+        <v>244</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>164</v>
+        <v>9</v>
       </c>
       <c r="G128" s="3"/>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B129" s="3"/>
-      <c r="C129" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G129" s="3"/>
-    </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B130" s="3"/>
+      <c r="B130" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="C130" s="1" t="s">
-        <v>166</v>
+        <v>63</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>162</v>
+        <v>50</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G130" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B131" s="3"/>
-      <c r="C131" s="1">
-        <v>4.5</v>
+      <c r="C131" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>171</v>
+        <v>9</v>
       </c>
       <c r="G131" s="3"/>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B132" s="3"/>
       <c r="C132" s="1" t="s">
-        <v>167</v>
+        <v>52</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>172</v>
+        <v>9</v>
       </c>
       <c r="G132" s="3"/>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B133" s="3"/>
       <c r="C133" s="1" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>173</v>
+        <v>9</v>
       </c>
       <c r="G133" s="3"/>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B134" s="3"/>
       <c r="C134" s="1" t="s">
-        <v>169</v>
+        <v>56</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>171</v>
+        <v>9</v>
       </c>
       <c r="G134" s="3"/>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B135" s="3"/>
       <c r="C135" s="1" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>174</v>
+        <v>9</v>
       </c>
       <c r="G135" s="3"/>
     </row>
     <row r="136" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B136" s="3"/>
       <c r="C136" s="1" t="s">
-        <v>176</v>
+        <v>57</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="G136" s="3"/>
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B137" s="3"/>
       <c r="C137" s="1" t="s">
-        <v>177</v>
+        <v>59</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="G137" s="3"/>
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B138" s="3"/>
       <c r="C138" s="1" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>178</v>
+        <v>9</v>
       </c>
       <c r="G138" s="3"/>
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B139" s="3"/>
       <c r="C139" s="1" t="s">
-        <v>185</v>
+        <v>61</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>180</v>
+        <v>9</v>
       </c>
       <c r="G139" s="3"/>
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B140" s="3"/>
       <c r="C140" s="1" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>181</v>
+        <v>9</v>
       </c>
       <c r="G140" s="3"/>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B141" s="3"/>
       <c r="C141" s="1" t="s">
-        <v>183</v>
+        <v>110</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
       <c r="G141" s="3"/>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B142" s="3"/>
       <c r="C142" s="1" t="s">
-        <v>201</v>
+        <v>139</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="G142" s="3"/>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B143" s="3"/>
       <c r="C143" s="1" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>156</v>
+        <v>264</v>
       </c>
       <c r="G143" s="3"/>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B144" s="3"/>
       <c r="C144" s="1" t="s">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>157</v>
+        <v>20</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>196</v>
+        <v>116</v>
       </c>
       <c r="G144" s="3"/>
     </row>
     <row r="145" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B145" s="3"/>
       <c r="C145" s="1" t="s">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>197</v>
+        <v>144</v>
       </c>
       <c r="G145" s="3"/>
     </row>
     <row r="146" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B146" s="3"/>
       <c r="C146" s="1" t="s">
-        <v>189</v>
+        <v>130</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="G146" s="3"/>
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B147" s="3"/>
       <c r="C147" s="1" t="s">
-        <v>190</v>
+        <v>128</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>156</v>
+        <v>44</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="G147" s="3"/>
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B148" s="3"/>
       <c r="C148" s="1" t="s">
-        <v>191</v>
+        <v>132</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="G148" s="3"/>
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B149" s="3"/>
       <c r="C149" s="1" t="s">
-        <v>192</v>
+        <v>134</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G149" s="3"/>
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B150" s="3"/>
       <c r="C150" s="1" t="s">
-        <v>193</v>
+        <v>133</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>199</v>
+        <v>119</v>
       </c>
       <c r="G150" s="3"/>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B151" s="3"/>
       <c r="C151" s="1" t="s">
-        <v>194</v>
+        <v>135</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="G151" s="3"/>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B152" s="3"/>
       <c r="C152" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G152" s="3"/>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B153" s="3"/>
+      <c r="C153" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G153" s="3"/>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B154" s="3"/>
+      <c r="C154" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G154" s="3"/>
+    </row>
+    <row r="156" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B156" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B157" s="3"/>
+      <c r="C157" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G157" s="3"/>
+    </row>
+    <row r="158" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B158" s="3"/>
+      <c r="C158" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G158" s="3"/>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B159" s="3"/>
+      <c r="C159" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G159" s="3"/>
+    </row>
+    <row r="160" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B160" s="3"/>
+      <c r="C160" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G160" s="3"/>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B161" s="3"/>
+      <c r="C161" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G161" s="3"/>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B162" s="3"/>
+      <c r="C162" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G162" s="3"/>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B163" s="3"/>
+      <c r="C163" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G163" s="3"/>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B164" s="3"/>
+      <c r="C164" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G164" s="3"/>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B165" s="3"/>
+      <c r="C165" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G165" s="3"/>
+    </row>
+    <row r="166" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B166" s="3"/>
+      <c r="C166" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G166" s="3"/>
+    </row>
+    <row r="167" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B167" s="3"/>
+      <c r="C167" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G167" s="3"/>
+    </row>
+    <row r="168" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B168" s="3"/>
+      <c r="C168" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G168" s="3"/>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B169" s="3"/>
+      <c r="C169" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G169" s="3"/>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B170" s="3"/>
+      <c r="C170" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G170" s="3"/>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B171" s="3"/>
+      <c r="C171" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G171" s="3"/>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B172" s="3"/>
+      <c r="C172" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G172" s="3"/>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B173" s="3"/>
+      <c r="C173" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G173" s="3"/>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B174" s="3"/>
+      <c r="C174" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G174" s="3"/>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B175" s="3"/>
+      <c r="C175" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G175" s="3"/>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B176" s="3"/>
+      <c r="C176" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G176" s="3"/>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B177" s="3"/>
+      <c r="C177" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G177" s="3"/>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B178" s="3"/>
+      <c r="C178" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G178" s="3"/>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B179" s="3"/>
+      <c r="C179" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G179" s="3"/>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B180" s="3"/>
+      <c r="C180" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G180" s="3"/>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B181" s="3"/>
+      <c r="C181" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G181" s="3"/>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B182" s="3"/>
+      <c r="C182" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G182" s="3"/>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B183" s="3"/>
+      <c r="C183" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G183" s="3"/>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B184" s="3"/>
+      <c r="C184" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G184" s="3"/>
+    </row>
+    <row r="185" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B185" s="3"/>
+      <c r="C185" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G185" s="3"/>
+    </row>
+    <row r="186" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B186" s="3"/>
+      <c r="C186" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G186" s="3"/>
+    </row>
+    <row r="187" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B187" s="3"/>
+      <c r="C187" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G187" s="3"/>
+    </row>
+    <row r="188" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B188" s="3"/>
+      <c r="C188" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G188" s="3"/>
+    </row>
+    <row r="189" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B189" s="3"/>
+      <c r="C189" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G189" s="3"/>
+    </row>
+    <row r="190" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B190" s="3"/>
+      <c r="C190" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G190" s="3"/>
+    </row>
+    <row r="191" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B191" s="3"/>
+      <c r="C191" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G191" s="3"/>
+    </row>
+    <row r="192" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B192" s="3"/>
+      <c r="C192" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G192" s="3"/>
+    </row>
+    <row r="193" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B193" s="3"/>
+      <c r="C193" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G193" s="3"/>
+    </row>
+    <row r="194" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B194" s="3"/>
+      <c r="C194" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G194" s="3"/>
+    </row>
+    <row r="195" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B195" s="3"/>
+      <c r="C195" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G195" s="3"/>
+    </row>
+    <row r="196" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B196" s="3"/>
+      <c r="C196" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G196" s="3"/>
+    </row>
+    <row r="197" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B197" s="3"/>
+      <c r="C197" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G197" s="3"/>
+    </row>
+    <row r="198" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B198" s="3"/>
+      <c r="C198" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G198" s="3"/>
+    </row>
+    <row r="199" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B199" s="3"/>
+      <c r="C199" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G199" s="3"/>
+    </row>
+    <row r="200" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B200" s="3"/>
+      <c r="C200" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G200" s="3"/>
+    </row>
+    <row r="201" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B201" s="3"/>
+      <c r="C201" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G201" s="3"/>
+    </row>
+    <row r="203" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B203" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G203" s="3"/>
+    </row>
+    <row r="204" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B204" s="3"/>
+      <c r="C204" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G204" s="3"/>
+    </row>
+    <row r="205" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B205" s="3"/>
+      <c r="C205" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G205" s="3"/>
+    </row>
+    <row r="206" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B206" s="3"/>
+      <c r="C206" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G206" s="3"/>
+    </row>
+    <row r="207" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B207" s="3"/>
+      <c r="C207" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G207" s="3"/>
+    </row>
+    <row r="208" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B208" s="3"/>
+      <c r="C208" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G208" s="3"/>
+    </row>
+    <row r="209" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B209" s="3"/>
+      <c r="C209" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G209" s="3"/>
+    </row>
+    <row r="210" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B210" s="3"/>
+      <c r="C210" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G210" s="3"/>
+    </row>
+    <row r="211" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B211" s="3"/>
+      <c r="C211" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G211" s="3"/>
+    </row>
+    <row r="212" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B212" s="3"/>
+      <c r="C212" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G212" s="3"/>
+    </row>
+    <row r="213" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B213" s="3"/>
+      <c r="C213" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G213" s="3"/>
+    </row>
+    <row r="214" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B214" s="3"/>
+      <c r="C214" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G214" s="3"/>
+    </row>
+    <row r="215" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B215" s="3"/>
+      <c r="C215" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G215" s="3"/>
+    </row>
+    <row r="216" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B216" s="3"/>
+      <c r="C216" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G216" s="3"/>
+    </row>
+    <row r="217" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B217" s="3"/>
+      <c r="C217" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G217" s="3"/>
+    </row>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B218" s="3"/>
+      <c r="C218" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G218" s="3"/>
+    </row>
+    <row r="219" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B219" s="3"/>
+      <c r="C219" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G219" s="3"/>
+    </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B220" s="3"/>
+      <c r="C220" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G220" s="3"/>
+    </row>
+    <row r="221" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B221" s="3"/>
+      <c r="C221" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G221" s="3"/>
+    </row>
+    <row r="222" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B222" s="3"/>
+      <c r="C222" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G222" s="3"/>
+    </row>
+    <row r="224" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B224" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G224" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="225" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B225" s="3"/>
+      <c r="C225" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G225" s="4"/>
+    </row>
+    <row r="226" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B226" s="3"/>
+      <c r="C226" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G226" s="4"/>
+    </row>
+    <row r="227" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B227" s="3"/>
+      <c r="C227" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G227" s="4"/>
+    </row>
+    <row r="228" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B228" s="3"/>
+      <c r="C228" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G228" s="4"/>
+    </row>
+    <row r="229" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B229" s="3"/>
+      <c r="C229" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G229" s="4"/>
+    </row>
+    <row r="230" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B230" s="3"/>
+      <c r="C230" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G230" s="4"/>
+    </row>
+    <row r="231" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B231" s="3"/>
+      <c r="C231" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G231" s="4"/>
+    </row>
+    <row r="232" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B232" s="3"/>
+      <c r="C232" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G232" s="4"/>
+    </row>
+    <row r="233" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B233" s="3"/>
+      <c r="C233" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G233" s="4"/>
+    </row>
+    <row r="234" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B234" s="3"/>
+      <c r="C234" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G234" s="4"/>
+    </row>
+    <row r="235" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B235" s="3"/>
+      <c r="C235" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G235" s="4"/>
+    </row>
+    <row r="236" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B236" s="3"/>
+      <c r="C236" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G236" s="4"/>
+    </row>
+    <row r="237" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B237" s="3"/>
+      <c r="C237" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G237" s="4"/>
+    </row>
+    <row r="238" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B238" s="3"/>
+      <c r="C238" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G238" s="4"/>
+    </row>
+    <row r="239" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B239" s="3"/>
+      <c r="C239" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G239" s="4"/>
+    </row>
+    <row r="240" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B240" s="3"/>
+      <c r="C240" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G240" s="4"/>
+    </row>
+    <row r="241" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B241" s="3"/>
+      <c r="C241" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G241" s="4"/>
+    </row>
+    <row r="242" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B242" s="3"/>
+      <c r="C242" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G242" s="4"/>
+    </row>
+    <row r="243" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B243" s="3"/>
+      <c r="C243" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G243" s="4"/>
+    </row>
+    <row r="244" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B244" s="3"/>
+      <c r="C244" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G244" s="4"/>
+    </row>
+    <row r="245" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B245" s="3"/>
+      <c r="C245" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G245" s="4"/>
+    </row>
+    <row r="246" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B246" s="3"/>
+      <c r="C246" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G246" s="4"/>
+    </row>
+    <row r="247" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B247" s="3"/>
+      <c r="C247" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G247" s="4"/>
+    </row>
+    <row r="248" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B248" s="3"/>
+      <c r="C248" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G248" s="4"/>
+    </row>
+    <row r="249" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B249" s="3"/>
+      <c r="C249" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G249" s="4"/>
+    </row>
+    <row r="250" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B250" s="3"/>
+      <c r="C250" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G250" s="4"/>
+    </row>
+    <row r="251" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B251" s="3"/>
+      <c r="C251" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G251" s="4"/>
+    </row>
+    <row r="252" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B252" s="3"/>
+      <c r="C252" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G252" s="4"/>
+    </row>
+    <row r="253" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B253" s="3"/>
+      <c r="C253" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G253" s="4"/>
+    </row>
+    <row r="254" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B254" s="3"/>
+      <c r="C254" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G254" s="4"/>
+    </row>
+    <row r="255" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B255" s="3"/>
+      <c r="C255" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G255" s="4"/>
+    </row>
+    <row r="256" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B256" s="3"/>
+      <c r="C256" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G256" s="4"/>
+    </row>
+    <row r="257" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B257" s="3"/>
+      <c r="C257" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G257" s="4"/>
+    </row>
+    <row r="258" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B258" s="3"/>
+      <c r="C258" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G258" s="4"/>
+    </row>
+    <row r="259" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B259" s="3"/>
+      <c r="C259" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G259" s="4"/>
+    </row>
+    <row r="260" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G260"/>
+    </row>
+    <row r="261" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G261"/>
+    </row>
+    <row r="262" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G262"/>
+    </row>
+    <row r="263" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G263"/>
+    </row>
+    <row r="264" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G264"/>
+    </row>
+    <row r="265" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G265"/>
+    </row>
+    <row r="266" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G266"/>
+    </row>
+    <row r="317" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B317" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F317" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="318" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C318" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F318" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="319" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C319" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F319" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="320" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C320" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F320" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="321" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C321" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F321" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="322" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C322" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F322" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="323" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C323" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D152" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F152" s="1" t="s">
+      <c r="D323" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E323" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F323" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="324" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C324" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E324" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F324" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="325" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C325" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E325" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F325" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="326" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C326" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E326" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F326" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="327" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C327" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G152" s="3"/>
-    </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B154" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C155" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C156" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C157" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C158" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C160" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C162" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C164" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C166" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B177" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C178" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C179" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C180" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F180" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C181" s="1" t="s">
+      <c r="D327" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E327" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F327" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="328" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C328" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E328" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F328" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="329" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C329" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E329" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F329" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="330" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C330" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D330" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F330" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D181" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C182" s="1" t="s">
+    </row>
+    <row r="331" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C331" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D331" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E331" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F331" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="332" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C332" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D332" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E332" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F332" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="333" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C333" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D182" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F182" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C183" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F183" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C184" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D184" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F184" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C185" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F185" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C186" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F186" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C187" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F187" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C188" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C189" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C190" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F190" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C191" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F191" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C192" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F192" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="193" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C193" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D193" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F193" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="194" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C194" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F194" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="195" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C195" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F195" s="1" t="s">
-        <v>156</v>
+      <c r="D333" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E333" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F333" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="334" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C334" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F334" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="335" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C335" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E335" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F335" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B110:B152"/>
-    <mergeCell ref="G110:G152"/>
+  <mergeCells count="26">
+    <mergeCell ref="B55:B68"/>
+    <mergeCell ref="G55:G68"/>
     <mergeCell ref="B4:B14"/>
     <mergeCell ref="B51:B53"/>
     <mergeCell ref="G21:G27"/>
@@ -3979,12 +5822,18 @@
     <mergeCell ref="B33:B49"/>
     <mergeCell ref="G4:G14"/>
     <mergeCell ref="G51:G53"/>
-    <mergeCell ref="G86:G108"/>
-    <mergeCell ref="B86:B108"/>
+    <mergeCell ref="G203:G222"/>
+    <mergeCell ref="B203:B222"/>
+    <mergeCell ref="B224:B259"/>
+    <mergeCell ref="G224:G259"/>
     <mergeCell ref="G70:G84"/>
     <mergeCell ref="B70:B84"/>
-    <mergeCell ref="B55:B68"/>
-    <mergeCell ref="G55:G68"/>
+    <mergeCell ref="B86:B128"/>
+    <mergeCell ref="G86:G128"/>
+    <mergeCell ref="B130:B154"/>
+    <mergeCell ref="G130:G154"/>
+    <mergeCell ref="B156:B201"/>
+    <mergeCell ref="G156:G201"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>